<commit_message>
Cris V1 20082022 V2
Fix Data Warehouse
</commit_message>
<xml_diff>
--- a/Desnormalización de la base de datos.xlsx
+++ b/Desnormalización de la base de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Proyecto-Data-WareHouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C21DF-F4B3-4CBF-8982-B4836BC36055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF44A4D-B193-409F-A0CA-8139B5A2FF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="-1050" windowWidth="16410" windowHeight="11835" xr2:uid="{C1B57FCB-8E1F-472F-B510-2EC42A2973EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C1B57FCB-8E1F-472F-B510-2EC42A2973EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Staging Area" sheetId="1" r:id="rId1"/>
@@ -313,15 +313,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7C5B2D-B036-413B-9827-29AD6B16810B}">
   <dimension ref="B2:AW8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU7" sqref="AU7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,74 +696,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9" t="s">
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9" t="s">
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9" t="s">
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9" t="s">
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
     </row>
     <row r="3" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -895,7 +895,7 @@
       <c r="AR3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AS3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="AT3" s="3" t="s">
@@ -930,7 +930,7 @@
       </c>
     </row>
     <row r="8" spans="2:49" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
@@ -958,7 +958,7 @@
   <dimension ref="B2:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,25 +985,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1054,7 +1054,7 @@
       <c r="Q3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1126,57 +1126,57 @@
       </c>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9" t="s">
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9" t="s">
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1274,12 +1274,12 @@
       </c>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1287,15 +1287,15 @@
       </c>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -1316,6 +1316,8 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AD2:AF2"/>
@@ -1326,8 +1328,6 @@
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>